<commit_message>
changes for different nomrlaization
Code and results for different normalization, aswell as code to check the results of the different normalization methods
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -75,7 +78,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Global and housekeeping modifications
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -81,7 +84,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
changes in globalT and HK
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,19 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>HK_G_acc_G</t>
-  </si>
-  <si>
-    <t>HK_G_acc_G</t>
-  </si>
-  <si>
-    <t>HK_G_acc_G</t>
-  </si>
-  <si>
-    <t>HK_G_acc_G</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -84,7 +72,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Clean for the global thersholding and solving rules
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -72,7 +81,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Do the ubiquity score
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -84,7 +93,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Changes for the ubiquity score
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -93,7 +99,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Finish the KH reactions thing
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -99,7 +102,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Plot with mean and not with one sample
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -102,7 +108,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
changes to obtain the new results
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -111,247 +114,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>50.810810810810814</v>
+        <v>51.179673321234119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>50.810810810810814</v>
+        <v>51.179673321234119</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>50.810810810810814</v>
+        <v>51.179673321234119</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>50.990990990990994</v>
+        <v>51.361161524500908</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>51.171171171171167</v>
+        <v>51.542649727767696</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>51.171171171171167</v>
+        <v>51.542649727767696</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>52.432432432432428</v>
+        <v>52.813067150635206</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>52.252252252252248</v>
+        <v>52.631578947368418</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>52.072072072072075</v>
+        <v>52.45009074410163</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>52.072072072072075</v>
+        <v>52.45009074410163</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>51.711711711711715</v>
+        <v>52.08711433756806</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>52.612612612612608</v>
+        <v>52.994555353901994</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>52.252252252252248</v>
+        <v>52.631578947368418</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>52.252252252252248</v>
+        <v>52.631578947368418</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>52.792792792792795</v>
+        <v>53.176043557168782</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>51.711711711711715</v>
+        <v>52.08711433756806</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>52.612612612612608</v>
+        <v>52.994555353901994</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>51.891891891891895</v>
+        <v>52.268602540834841</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>51.711711711711715</v>
+        <v>52.08711433756806</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>51.711711711711715</v>
+        <v>52.08711433756806</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>51.891891891891895</v>
+        <v>52.268602540834841</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>50.090090090090087</v>
+        <v>50.453720508166967</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>49.009009009009006</v>
+        <v>49.364791288566245</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>49.369369369369373</v>
+        <v>49.727767695099814</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>51.531531531531527</v>
+        <v>51.905626134301272</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>51.531531531531527</v>
+        <v>51.905626134301272</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>52.252252252252248</v>
+        <v>52.631578947368418</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>53.153153153153156</v>
+        <v>53.539019963702358</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>52.432432432432428</v>
+        <v>52.813067150635206</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>52.792792792792795</v>
+        <v>53.176043557168782</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>49.729729729729733</v>
+        <v>50.090744101633391</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>50.270270270270267</v>
+        <v>50.635208711433755</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>50.450450450450447</v>
+        <v>50.816696914700543</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>51.171171171171167</v>
+        <v>51.542649727767696</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>51.171171171171167</v>
+        <v>51.542649727767696</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>56.396396396396398</v>
+        <v>56.805807622504531</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>49.729729729729733</v>
+        <v>50.090744101633391</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>50.810810810810814</v>
+        <v>51.179673321234119</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>50.810810810810814</v>
+        <v>51.179673321234119</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>52.252252252252248</v>
+        <v>52.631578947368418</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>52.072072072072075</v>
+        <v>52.45009074410163</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>52.972972972972975</v>
+        <v>53.35753176043557</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>52.612612612612608</v>
+        <v>52.994555353901994</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>50.990990990990994</v>
+        <v>51.361161524500908</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>50.990990990990994</v>
+        <v>51.361161524500908</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>50.630630630630634</v>
+        <v>50.998185117967331</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>54.054054054054056</v>
+        <v>54.446460980036292</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>51.711711711711715</v>
+        <v>52.08711433756806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes with different HK_datasets
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -114,247 +120,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>51.179673321234119</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>51.179673321234119</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>51.179673321234119</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>51.361161524500908</v>
+        <v>71.481481481481481</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>51.542649727767696</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>51.542649727767696</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>52.813067150635206</v>
+        <v>73.703703703703709</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>52.631578947368418</v>
+        <v>74.074074074074076</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>52.45009074410163</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>52.45009074410163</v>
+        <v>74.074074074074076</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>52.08711433756806</v>
+        <v>72.592592592592595</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>52.994555353901994</v>
+        <v>73.333333333333329</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>52.631578947368418</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>52.631578947368418</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>53.176043557168782</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>52.08711433756806</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>52.994555353901994</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>52.268602540834841</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>52.08711433756806</v>
+        <v>73.333333333333329</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>52.08711433756806</v>
+        <v>73.703703703703709</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>52.268602540834841</v>
+        <v>74.074074074074076</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>50.453720508166967</v>
+        <v>70.370370370370367</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>49.364791288566245</v>
+        <v>70.370370370370367</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>49.727767695099814</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>51.905626134301272</v>
+        <v>73.333333333333329</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>51.905626134301272</v>
+        <v>72.962962962962962</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>52.631578947368418</v>
+        <v>74.074074074074076</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>53.539019963702358</v>
+        <v>75.18518518518519</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>52.813067150635206</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>53.176043557168782</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>50.090744101633391</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>50.635208711433755</v>
+        <v>70.370370370370367</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>50.816696914700543</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>51.542649727767696</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>51.542649727767696</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>56.805807622504531</v>
+        <v>75.925925925925924</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>50.090744101633391</v>
+        <v>69.259259259259252</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>51.179673321234119</v>
+        <v>69.629629629629633</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>51.179673321234119</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>52.631578947368418</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>52.45009074410163</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>53.35753176043557</v>
+        <v>75.18518518518519</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>52.994555353901994</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>51.361161524500908</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>51.361161524500908</v>
+        <v>71.481481481481481</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>50.998185117967331</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>54.446460980036292</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>52.08711433756806</v>
+        <v>71.111111111111114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the mean calculation to the sample datasets
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -112,7 +148,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A49"/>
+  <dimension ref="A1:A50"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="true"/>
@@ -120,247 +156,252 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>71.851851851851862</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>71.851851851851862</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>71.851851851851862</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>71.481481481481481</v>
+        <v>71.217712177121768</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>71.851851851851862</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>71.851851851851862</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>73.703703703703709</v>
+        <v>73.431734317343171</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>74.074074074074076</v>
+        <v>73.800738007380076</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>74.81481481481481</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>74.074074074074076</v>
+        <v>73.800738007380076</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>72.592592592592595</v>
+        <v>72.32472324723247</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>73.333333333333329</v>
+        <v>73.062730627306266</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>74.81481481481481</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>74.81481481481481</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>74.81481481481481</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>74.444444444444443</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>74.444444444444443</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>74.81481481481481</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>73.333333333333329</v>
+        <v>73.062730627306266</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>73.703703703703709</v>
+        <v>73.431734317343171</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>74.074074074074076</v>
+        <v>73.800738007380076</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>70.370370370370367</v>
+        <v>70.110701107011081</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>70.370370370370367</v>
+        <v>70.110701107011081</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>70</v>
+        <v>69.741697416974162</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>73.333333333333329</v>
+        <v>73.062730627306266</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>72.962962962962962</v>
+        <v>72.693726937269375</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>74.074074074074076</v>
+        <v>73.800738007380076</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>75.18518518518519</v>
+        <v>74.907749077490777</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>74.81481481481481</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>74.444444444444443</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>70</v>
+        <v>69.741697416974162</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>70.370370370370367</v>
+        <v>70.110701107011081</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>71.851851851851862</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>70.740740740740733</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>70.740740740740733</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>75.925925925925924</v>
+        <v>75.645756457564573</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>69.259259259259252</v>
+        <v>69.003690036900366</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>69.629629629629633</v>
+        <v>69.372693726937271</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>70.740740740740733</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>74.444444444444443</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>74.444444444444443</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>75.18518518518519</v>
+        <v>74.907749077490777</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>74.444444444444443</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>70.740740740740733</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>71.481481481481481</v>
+        <v>71.217712177121768</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>70.740740740740733</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>74.81481481481481</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>71.111111111111114</v>
+        <v>70.848708487084863</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>73.431734317343171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve in the Global_Thresholding comments
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -156,7 +159,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Results with new HKlist
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -159,252 +165,252 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>71.586715867158674</v>
+        <v>48.141891891891895</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>71.586715867158674</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>71.586715867158674</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>71.217712177121768</v>
+        <v>47.804054054054049</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>71.586715867158674</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>71.586715867158674</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>73.431734317343171</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>73.800738007380076</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>74.538745387453872</v>
+        <v>48.648648648648653</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>73.800738007380076</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>72.32472324723247</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>73.062730627306266</v>
+        <v>49.831081081081081</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>74.538745387453872</v>
+        <v>49.662162162162161</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>74.538745387453872</v>
+        <v>50.168918918918912</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>74.538745387453872</v>
+        <v>50.168918918918912</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>74.169741697416967</v>
+        <v>50.506756756756758</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>74.169741697416967</v>
+        <v>51.013513513513509</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>74.538745387453872</v>
+        <v>50.844594594594597</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>73.062730627306266</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>73.431734317343171</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>73.800738007380076</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>70.110701107011081</v>
+        <v>47.297297297297298</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>70.110701107011081</v>
+        <v>46.95945945945946</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>69.741697416974162</v>
+        <v>46.95945945945946</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>73.062730627306266</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>72.693726937269375</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>73.800738007380076</v>
+        <v>49.324324324324323</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>74.907749077490777</v>
+        <v>50.168918918918912</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>74.538745387453872</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>74.169741697416967</v>
+        <v>49.493243243243242</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>69.741697416974162</v>
+        <v>47.466216216216218</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>70.110701107011081</v>
+        <v>46.95945945945946</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>71.586715867158674</v>
+        <v>47.804054054054049</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>70.479704797047972</v>
+        <v>47.635135135135137</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>70.479704797047972</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>75.645756457564573</v>
+        <v>51.520270270270274</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>69.003690036900366</v>
+        <v>47.466216216216218</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>69.372693726937271</v>
+        <v>47.635135135135137</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>70.479704797047972</v>
+        <v>47.972972972972968</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>74.169741697416967</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>74.169741697416967</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>74.907749077490777</v>
+        <v>49.831081081081081</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>74.169741697416967</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>70.479704797047972</v>
+        <v>48.141891891891895</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>71.217712177121768</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>70.479704797047972</v>
+        <v>48.141891891891895</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>74.538745387453872</v>
+        <v>51.351351351351347</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>70.848708487084863</v>
+        <v>49.324324324324323</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>73.431734317343171</v>
+        <v>49.493243243243242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plots with standard deviation
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -165,7 +174,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
changes in context model and in the plots
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -174,7 +177,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Changes to obtain the subSystems of HKR
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -195,252 +198,252 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>71.586715867158674</v>
+        <v>48.141891891891895</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>71.586715867158674</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>71.586715867158674</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>71.217712177121768</v>
+        <v>47.804054054054049</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>71.586715867158674</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>71.586715867158674</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>73.431734317343171</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>73.800738007380076</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>74.538745387453872</v>
+        <v>48.648648648648653</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>73.800738007380076</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>72.32472324723247</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>73.062730627306266</v>
+        <v>49.831081081081081</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>74.538745387453872</v>
+        <v>49.662162162162161</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>74.538745387453872</v>
+        <v>50.168918918918912</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>74.538745387453872</v>
+        <v>50.168918918918912</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>74.169741697416967</v>
+        <v>50.506756756756758</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>74.169741697416967</v>
+        <v>51.013513513513509</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>74.538745387453872</v>
+        <v>50.844594594594597</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>73.062730627306266</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>73.431734317343171</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>73.800738007380076</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>70.110701107011081</v>
+        <v>47.297297297297298</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>70.110701107011081</v>
+        <v>46.95945945945946</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>69.741697416974162</v>
+        <v>46.95945945945946</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>73.062730627306266</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>72.693726937269375</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>73.800738007380076</v>
+        <v>49.324324324324323</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>74.907749077490777</v>
+        <v>50.168918918918912</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>74.538745387453872</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>74.169741697416967</v>
+        <v>49.493243243243242</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>69.741697416974162</v>
+        <v>47.466216216216218</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>70.110701107011081</v>
+        <v>46.95945945945946</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>71.586715867158674</v>
+        <v>47.804054054054049</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>70.479704797047972</v>
+        <v>47.635135135135137</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>70.479704797047972</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>75.645756457564573</v>
+        <v>51.520270270270274</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>69.003690036900366</v>
+        <v>47.466216216216218</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>69.372693726937271</v>
+        <v>47.635135135135137</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>70.479704797047972</v>
+        <v>47.972972972972968</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>74.169741697416967</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>74.169741697416967</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>74.907749077490777</v>
+        <v>49.831081081081081</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>74.169741697416967</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>70.479704797047972</v>
+        <v>48.141891891891895</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>71.217712177121768</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>70.479704797047972</v>
+        <v>48.141891891891895</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>74.538745387453872</v>
+        <v>51.351351351351347</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>70.848708487084863</v>
+        <v>49.324324324324323</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>73.431734317343171</v>
+        <v>49.493243243243242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in global, changes in teh enzyme thing
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -198,252 +201,252 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>48.141891891891895</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>48.310810810810814</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>48.479729729729733</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>47.804054054054049</v>
+        <v>71.217712177121768</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>48.310810810810814</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>48.310810810810814</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>48.986486486486484</v>
+        <v>73.431734317343171</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>49.155405405405403</v>
+        <v>73.800738007380076</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>48.648648648648653</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>48.479729729729733</v>
+        <v>73.800738007380076</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>48.986486486486484</v>
+        <v>72.32472324723247</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>49.831081081081081</v>
+        <v>73.062730627306266</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>49.662162162162161</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>50.168918918918912</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>50.168918918918912</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>50.506756756756758</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>51.013513513513509</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>50.844594594594597</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>48.986486486486484</v>
+        <v>73.062730627306266</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>49.155405405405403</v>
+        <v>73.431734317343171</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>48.986486486486484</v>
+        <v>73.800738007380076</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>47.297297297297298</v>
+        <v>70.110701107011081</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>46.95945945945946</v>
+        <v>70.110701107011081</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>46.95945945945946</v>
+        <v>69.741697416974162</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>48.479729729729733</v>
+        <v>73.062730627306266</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>48.479729729729733</v>
+        <v>72.693726937269375</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>49.324324324324323</v>
+        <v>73.800738007380076</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>50.168918918918912</v>
+        <v>74.907749077490777</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>50</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>49.493243243243242</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>47.466216216216218</v>
+        <v>69.741697416974162</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>46.95945945945946</v>
+        <v>70.110701107011081</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>47.804054054054049</v>
+        <v>71.586715867158674</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>47.635135135135137</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>48.310810810810814</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>51.520270270270274</v>
+        <v>75.645756457564573</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>47.466216216216218</v>
+        <v>69.003690036900366</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>47.635135135135137</v>
+        <v>69.372693726937271</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>47.972972972972968</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>49.155405405405403</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>48.479729729729733</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>49.831081081081081</v>
+        <v>74.907749077490777</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>49.155405405405403</v>
+        <v>74.169741697416967</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>48.141891891891895</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>48.310810810810814</v>
+        <v>71.217712177121768</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>48.141891891891895</v>
+        <v>70.479704797047972</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>51.351351351351347</v>
+        <v>74.538745387453872</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>49.324324324324323</v>
+        <v>70.848708487084863</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>49.493243243243242</v>
+        <v>73.431734317343171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculate the mean in the GloblaThesholding
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -201,247 +225,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>71.586715867158674</v>
+        <v>48.141891891891895</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>71.586715867158674</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>71.586715867158674</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>71.217712177121768</v>
+        <v>47.804054054054049</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>71.586715867158674</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>71.586715867158674</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>73.431734317343171</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>73.800738007380076</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>74.538745387453872</v>
+        <v>48.648648648648653</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>73.800738007380076</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>72.32472324723247</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>73.062730627306266</v>
+        <v>49.831081081081081</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>74.538745387453872</v>
+        <v>49.662162162162161</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>74.538745387453872</v>
+        <v>50.168918918918912</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>74.538745387453872</v>
+        <v>50.168918918918912</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>74.169741697416967</v>
+        <v>50.506756756756758</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>74.169741697416967</v>
+        <v>51.013513513513509</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>74.538745387453872</v>
+        <v>50.844594594594597</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>73.062730627306266</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>73.431734317343171</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>73.800738007380076</v>
+        <v>48.986486486486484</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>70.110701107011081</v>
+        <v>47.297297297297298</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>70.110701107011081</v>
+        <v>46.95945945945946</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>69.741697416974162</v>
+        <v>46.95945945945946</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>73.062730627306266</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>72.693726937269375</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>73.800738007380076</v>
+        <v>49.324324324324323</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>74.907749077490777</v>
+        <v>50.168918918918912</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>74.538745387453872</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>74.169741697416967</v>
+        <v>49.493243243243242</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>69.741697416974162</v>
+        <v>47.466216216216218</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>70.110701107011081</v>
+        <v>46.95945945945946</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>71.586715867158674</v>
+        <v>47.804054054054049</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>70.479704797047972</v>
+        <v>47.635135135135137</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>70.479704797047972</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>75.645756457564573</v>
+        <v>51.520270270270274</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>69.003690036900366</v>
+        <v>47.466216216216218</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>69.372693726937271</v>
+        <v>47.635135135135137</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>70.479704797047972</v>
+        <v>47.972972972972968</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>74.169741697416967</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>74.169741697416967</v>
+        <v>48.479729729729733</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>74.907749077490777</v>
+        <v>49.831081081081081</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>74.169741697416967</v>
+        <v>49.155405405405403</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>70.479704797047972</v>
+        <v>48.141891891891895</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>71.217712177121768</v>
+        <v>48.310810810810814</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>70.479704797047972</v>
+        <v>48.141891891891895</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>74.538745387453872</v>
+        <v>51.351351351351347</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>70.848708487084863</v>
+        <v>49.324324324324323</v>
       </c>
     </row>
     <row r="50">

</xml_diff>

<commit_message>
Solved the COBRAToolbox problem
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -225,7 +237,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Plot solved for LocalT2
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -237,7 +240,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Delete the cobratoolbox and changes
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="59" uniqueCount="58">
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -231,11 +231,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="1" max="1" width="11.453125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Code with the same core set sizes
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="6" uniqueCount="1">
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -77,242 +77,242 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>48.141891891891895</v>
+        <v>87.331081081081081</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>48.310810810810814</v>
+        <v>86.993243243243242</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>48.479729729729733</v>
+        <v>87.331081081081081</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>47.804054054054049</v>
+        <v>86.317567567567565</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>48.310810810810814</v>
+        <v>86.148648648648646</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>48.310810810810814</v>
+        <v>86.317567567567565</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>48.986486486486484</v>
+        <v>87.331081081081081</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>49.155405405405403</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>48.648648648648653</v>
+        <v>87.837837837837839</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>48.479729729729733</v>
+        <v>87.668918918918919</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>48.986486486486484</v>
+        <v>86.824324324324323</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>49.831081081081081</v>
+        <v>86.486486486486484</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>49.662162162162161</v>
+        <v>86.824324324324323</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>50.168918918918912</v>
+        <v>87.331081081081081</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>50.168918918918912</v>
+        <v>87.162162162162161</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>50.506756756756758</v>
+        <v>86.655405405405403</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>51.013513513513509</v>
+        <v>87.162162162162161</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>50.844594594594597</v>
+        <v>86.317567567567565</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>48.986486486486484</v>
+        <v>87.331081081081081</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>49.155405405405403</v>
+        <v>87.331081081081081</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>48.986486486486484</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>47.297297297297298</v>
+        <v>86.148648648648646</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>46.95945945945946</v>
+        <v>85.979729729729726</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>46.95945945945946</v>
+        <v>85.641891891891902</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>48.479729729729733</v>
+        <v>86.486486486486484</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>48.479729729729733</v>
+        <v>86.148648648648646</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>49.324324324324323</v>
+        <v>86.486486486486484</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>50.168918918918912</v>
+        <v>87.162162162162161</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>50</v>
+        <v>87.331081081081081</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>49.493243243243242</v>
+        <v>86.824324324324323</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>47.466216216216218</v>
+        <v>86.655405405405403</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>46.95945945945946</v>
+        <v>86.824324324324323</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>47.804054054054049</v>
+        <v>86.824324324324323</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>47.635135135135137</v>
+        <v>86.824324324324323</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>48.310810810810814</v>
+        <v>86.824324324324323</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>51.520270270270274</v>
+        <v>88.175675675675677</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>47.466216216216218</v>
+        <v>86.317567567567565</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>47.635135135135137</v>
+        <v>86.993243243243242</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>47.972972972972968</v>
+        <v>86.486486486486484</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>49.155405405405403</v>
+        <v>86.655405405405403</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>48.479729729729733</v>
+        <v>86.486486486486484</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>49.831081081081081</v>
+        <v>86.317567567567565</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>49.155405405405403</v>
+        <v>86.655405405405403</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>48.141891891891895</v>
+        <v>86.824324324324323</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>48.310810810810814</v>
+        <v>86.655405405405403</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>48.141891891891895</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>51.351351351351347</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>49.324324324324323</v>
+        <v>87.668918918918919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>